<commit_message>
LV_T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton - Initial - 14 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
+++ b/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngoyal0630\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F1EA42-02E2-4006-860D-7A8B7F63ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7410" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>CompanyName</t>
   </si>
@@ -61,9 +62,6 @@
     <t>MailingState</t>
   </si>
   <si>
-    <t>StandardTestCompany</t>
-  </si>
-  <si>
     <t>Kansas</t>
   </si>
   <si>
@@ -106,9 +104,6 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Super</t>
-  </si>
-  <si>
     <t>Test Street 1</t>
   </si>
   <si>
@@ -121,9 +116,6 @@
     <t>Street 3</t>
   </si>
   <si>
-    <t>Test Street 3</t>
-  </si>
-  <si>
     <t>LP</t>
   </si>
   <si>
@@ -133,9 +125,6 @@
     <t>PU</t>
   </si>
   <si>
-    <t>NP</t>
-  </si>
-  <si>
     <t>Distribution Lists</t>
   </si>
   <si>
@@ -148,9 +137,6 @@
     <t>Washington</t>
   </si>
   <si>
-    <t>Florida</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -181,15 +167,6 @@
     <t>United States</t>
   </si>
   <si>
-    <t>External Contacts</t>
-  </si>
-  <si>
-    <t>Houlihan Employees</t>
-  </si>
-  <si>
-    <t>Distribution List</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -214,9 +191,6 @@
     <t>testSample@email.com</t>
   </si>
   <si>
-    <t>testingSuper@email.com</t>
-  </si>
-  <si>
     <t>FVA</t>
   </si>
   <si>
@@ -260,12 +234,21 @@
   </si>
   <si>
     <t>Operating Company</t>
+  </si>
+  <si>
+    <t>ActivityCompany</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>Conflicts Check LDCCR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,8 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -587,34 +569,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,72 +607,72 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="F2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -699,197 +681,165 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>39</v>
+      <c r="J6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -898,23 +848,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -923,29 +871,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>74</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -954,31 +905,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>68</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -987,26 +938,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>70</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1015,51 +966,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mid - LV_T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton - 14 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
+++ b/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F1EA42-02E2-4006-860D-7A8B7F63ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9107E54E-A57E-428F-BBAB-51198B4B8389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>CompanyName</t>
   </si>
@@ -98,45 +98,21 @@
     <t>Bingo</t>
   </si>
   <si>
-    <t>Jammer</t>
-  </si>
-  <si>
-    <t>Sample</t>
-  </si>
-  <si>
     <t>Test Street 1</t>
   </si>
   <si>
     <t>Street 2</t>
   </si>
   <si>
-    <t>Test Street 2</t>
-  </si>
-  <si>
-    <t>Street 3</t>
-  </si>
-  <si>
     <t>LP</t>
   </si>
   <si>
-    <t>TS</t>
-  </si>
-  <si>
-    <t>PU</t>
-  </si>
-  <si>
     <t>Distribution Lists</t>
   </si>
   <si>
     <t>New York</t>
   </si>
   <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -185,24 +161,9 @@
     <t>testBingo@email.com</t>
   </si>
   <si>
-    <t>testingJammer@email.com</t>
-  </si>
-  <si>
-    <t>testSample@email.com</t>
-  </si>
-  <si>
-    <t>FVA</t>
-  </si>
-  <si>
     <t>LineOfBusiness</t>
   </si>
   <si>
-    <t>ProjectNotifyRole</t>
-  </si>
-  <si>
-    <t>AR_FVA_FF</t>
-  </si>
-  <si>
     <t>UsersType</t>
   </si>
   <si>
@@ -218,15 +179,9 @@
     <t>Jennie Baker</t>
   </si>
   <si>
-    <t>Mentor</t>
-  </si>
-  <si>
     <t>Associate</t>
   </si>
   <si>
-    <t>Sonika Goyal</t>
-  </si>
-  <si>
     <t>CompanyType</t>
   </si>
   <si>
@@ -239,10 +194,22 @@
     <t>ActivityCompany</t>
   </si>
   <si>
-    <t>Archived</t>
-  </si>
-  <si>
-    <t>Conflicts Check LDCCR</t>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Test CK Summer</t>
+  </si>
+  <si>
+    <t>Testing PS Winter</t>
+  </si>
+  <si>
+    <t>Test LP Bingo</t>
+  </si>
+  <si>
+    <t>PinCode</t>
   </si>
 </sst>
 </file>
@@ -570,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,19 +548,18 @@
     <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -607,57 +573,57 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -666,57 +632,57 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>11</v>
-      </c>
-      <c r="K2" t="s">
-        <v>44</v>
       </c>
       <c r="L2" t="s">
         <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="S2">
+        <v>92001</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -725,30 +691,57 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
+      <c r="Q3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3">
+        <v>92001</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -757,89 +750,52 @@
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
       </c>
       <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4">
+        <v>92001</v>
       </c>
     </row>
   </sheetData>
@@ -885,18 +841,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -919,17 +875,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -952,12 +908,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -967,10 +923,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,21 +946,11 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LV_T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton - Final - 15 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
+++ b/TestData/T1063_Contacts_AddMultipleContactsToAnExistingCompanyAndValidateSaveAndNewButton.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D8D60-EEE6-4BB1-A3CE-6BE23718E01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3902021E-D5CA-4048-96BF-33050D104724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>CompanyName</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>HR</t>
   </si>
   <si>
     <t>User</t>
@@ -533,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -572,7 +569,7 @@
         <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -608,12 +605,12 @@
         <v>41</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -628,7 +625,7 @@
         <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -655,13 +652,13 @@
         <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R2">
         <v>92001</v>
@@ -669,7 +666,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -684,7 +681,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
@@ -711,13 +708,13 @@
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R3">
         <v>92001</v>
@@ -725,7 +722,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -740,7 +737,7 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
         <v>19</v>
@@ -767,13 +764,13 @@
         <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R4">
         <v>92001</v>
@@ -822,18 +819,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -843,10 +840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,11 +859,6 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -889,12 +881,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>